<commit_message>
Version submitted for grading
</commit_message>
<xml_diff>
--- a/Homework2/Results/time.xlsx
+++ b/Homework2/Results/time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="12">
   <si>
     <t>LinkedList</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>u-sec</t>
+  </si>
+  <si>
+    <t>Data Size</t>
   </si>
 </sst>
 </file>
@@ -587,6 +590,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time per Element</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1199,6 +1220,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time per Element</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2067,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2080,9 +2119,10 @@
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2101,8 +2141,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2124,8 +2167,12 @@
         <f>E2*10^6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f>D2*4</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2147,8 +2194,12 @@
         <f t="shared" ref="F3:F66" si="2">E3*10^6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="3">D3*4</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2170,8 +2221,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2193,8 +2248,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2216,8 +2275,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2239,8 +2302,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2262,8 +2329,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2285,8 +2356,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2308,8 +2383,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2331,8 +2410,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2354,8 +2437,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2377,8 +2464,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2400,8 +2491,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2423,8 +2518,12 @@
         <f t="shared" si="2"/>
         <v>3.814697265625</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2446,8 +2545,12 @@
         <f t="shared" si="2"/>
         <v>3.814697265625</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2469,8 +2572,12 @@
         <f t="shared" si="2"/>
         <v>3.814697265625</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2492,8 +2599,12 @@
         <f t="shared" si="2"/>
         <v>3.337860107421875</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2515,8 +2626,12 @@
         <f t="shared" si="2"/>
         <v>3.5762786865234375</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2538,8 +2653,12 @@
         <f t="shared" si="2"/>
         <v>3.5762786865234375</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2561,8 +2680,12 @@
         <f t="shared" si="2"/>
         <v>3.5762786865234375</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2584,8 +2707,12 @@
         <f t="shared" si="2"/>
         <v>3.6358833312988281</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2607,8 +2734,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2630,8 +2761,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2653,8 +2788,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2676,8 +2815,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2699,8 +2842,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2722,8 +2869,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2745,8 +2896,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2768,8 +2923,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -2791,8 +2950,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2814,8 +2977,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2837,8 +3004,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2860,8 +3031,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -2883,8 +3058,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2906,8 +3085,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -2929,8 +3112,12 @@
         <f t="shared" si="2"/>
         <v>1.9073486328125</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2952,8 +3139,12 @@
         <f t="shared" si="2"/>
         <v>0.95367431640625</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -2975,8 +3166,12 @@
         <f t="shared" si="2"/>
         <v>1.430511474609375</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -2998,8 +3193,12 @@
         <f t="shared" si="2"/>
         <v>1.6689300537109375</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -3021,8 +3220,12 @@
         <f t="shared" si="2"/>
         <v>1.5497207641601563</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <f t="shared" si="3"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -3044,8 +3247,12 @@
         <f t="shared" si="2"/>
         <v>1.6689300537109375</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -3067,8 +3274,12 @@
         <f t="shared" si="2"/>
         <v>1.7285346984863281</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <f t="shared" si="3"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -3090,8 +3301,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -3113,8 +3328,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3136,8 +3355,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3159,8 +3382,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <f t="shared" si="3"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3182,8 +3409,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3205,8 +3436,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3228,8 +3463,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <f t="shared" si="3"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3251,8 +3490,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <f t="shared" si="3"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3274,8 +3517,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <f t="shared" si="3"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3297,8 +3544,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <f t="shared" si="3"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3320,8 +3571,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <f t="shared" si="3"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3343,8 +3598,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <f t="shared" si="3"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3366,8 +3625,12 @@
         <f t="shared" si="2"/>
         <v>7.62939453125</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <f t="shared" si="3"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3389,8 +3652,12 @@
         <f t="shared" si="2"/>
         <v>11.444091796875</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <f t="shared" si="3"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3412,8 +3679,12 @@
         <f t="shared" si="2"/>
         <v>15.2587890625</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <f t="shared" si="3"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3435,8 +3706,12 @@
         <f t="shared" si="2"/>
         <v>20.02716064453125</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <f t="shared" si="3"/>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -3458,8 +3733,12 @@
         <f t="shared" si="2"/>
         <v>37.19329833984375</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <f t="shared" si="3"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3481,8 +3760,12 @@
         <f t="shared" si="2"/>
         <v>60.319900512695313</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <f t="shared" si="3"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3504,8 +3787,12 @@
         <f t="shared" si="2"/>
         <v>71.763992309570313</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <f t="shared" si="3"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -3527,8 +3814,12 @@
         <f t="shared" si="2"/>
         <v>81.06231689453125</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <f t="shared" si="3"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -3550,8 +3841,12 @@
         <f t="shared" si="2"/>
         <v>89.168548583984375</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <f t="shared" si="3"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -3573,8 +3868,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -3596,8 +3895,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <f t="shared" si="3"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -3608,19 +3911,23 @@
         <v>0</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D106" si="3">POWER(2,B67)</f>
+        <f t="shared" ref="D67:D106" si="4">POWER(2,B67)</f>
         <v>128</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E106" si="4">C67/D67</f>
+        <f t="shared" ref="E67:E106" si="5">C67/D67</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F106" si="5">E67*10^6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <f t="shared" ref="F67:F106" si="6">E67*10^6</f>
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G106" si="7">D67*4</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -3631,19 +3938,23 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="E68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F68">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -3654,19 +3965,23 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="E69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F69">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="7"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -3677,19 +3992,23 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="E70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F70">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="7"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -3700,19 +4019,23 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="E71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="7"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -3723,19 +4046,23 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="E72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -3746,19 +4073,23 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="E73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="7"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -3769,19 +4100,23 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16384</v>
       </c>
       <c r="E74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F74">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="7"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -3792,19 +4127,23 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32768</v>
       </c>
       <c r="E75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F75">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="7"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -3815,19 +4154,23 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65536</v>
       </c>
       <c r="E76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F76">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -3838,19 +4181,23 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131072</v>
       </c>
       <c r="E77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="7"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -3861,19 +4208,23 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>262144</v>
       </c>
       <c r="E78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F78">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="7"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -3884,19 +4235,23 @@
         <v>1</v>
       </c>
       <c r="D79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>524288</v>
       </c>
       <c r="E79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9073486328125E-6</v>
       </c>
       <c r="F79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9073486328125</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <f t="shared" si="7"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -3907,19 +4262,23 @@
         <v>1</v>
       </c>
       <c r="D80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1048576</v>
       </c>
       <c r="E80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5367431640625E-7</v>
       </c>
       <c r="F80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.95367431640625</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -3930,19 +4289,23 @@
         <v>3</v>
       </c>
       <c r="D81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2097152</v>
       </c>
       <c r="E81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.430511474609375E-6</v>
       </c>
       <c r="F81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.430511474609375</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <f t="shared" si="7"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -3953,19 +4316,23 @@
         <v>7</v>
       </c>
       <c r="D82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
       <c r="E82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6689300537109375E-6</v>
       </c>
       <c r="F82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6689300537109375</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <f t="shared" si="7"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -3976,19 +4343,23 @@
         <v>13</v>
       </c>
       <c r="D83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8388608</v>
       </c>
       <c r="E83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5497207641601563E-6</v>
       </c>
       <c r="F83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5497207641601563</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <f t="shared" si="7"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -3999,19 +4370,23 @@
         <v>27</v>
       </c>
       <c r="D84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16777216</v>
       </c>
       <c r="E84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6093254089355469E-6</v>
       </c>
       <c r="F84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6093254089355469</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <f t="shared" si="7"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -4022,19 +4397,23 @@
         <v>55</v>
       </c>
       <c r="D85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33554432</v>
       </c>
       <c r="E85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6391277313232422E-6</v>
       </c>
       <c r="F85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6391277313232422</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <f t="shared" si="7"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -4045,19 +4424,23 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="E86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F86">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -4068,19 +4451,23 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="E87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F87">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -4091,19 +4478,23 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="E88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F88">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="7"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -4114,19 +4505,23 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="E89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F89">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="7"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -4137,19 +4532,23 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="E90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F90">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="7"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -4160,19 +4559,23 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="E91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F91">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="7"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -4183,19 +4586,23 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="E92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F92">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="7"/>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -4206,19 +4613,23 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="E93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F93">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="7"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -4229,19 +4640,23 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="E94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F94">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="7"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>4</v>
       </c>
@@ -4252,19 +4667,23 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16384</v>
       </c>
       <c r="E95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F95">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="7"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -4275,19 +4694,23 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32768</v>
       </c>
       <c r="E96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F96">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <f t="shared" si="7"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -4298,19 +4721,23 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65536</v>
       </c>
       <c r="E97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F97">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="7"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -4321,19 +4748,23 @@
         <v>0</v>
       </c>
       <c r="D98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131072</v>
       </c>
       <c r="E98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F98">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="7"/>
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -4344,19 +4775,23 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>262144</v>
       </c>
       <c r="E99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F99">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="7"/>
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -4367,19 +4802,23 @@
         <v>1</v>
       </c>
       <c r="D100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>524288</v>
       </c>
       <c r="E100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9073486328125E-6</v>
       </c>
       <c r="F100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9073486328125</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <f t="shared" si="7"/>
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -4390,19 +4829,23 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1048576</v>
       </c>
       <c r="E101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5367431640625E-7</v>
       </c>
       <c r="F101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.95367431640625</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -4413,19 +4856,23 @@
         <v>4</v>
       </c>
       <c r="D102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2097152</v>
       </c>
       <c r="E102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9073486328125E-6</v>
       </c>
       <c r="F102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9073486328125</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <f t="shared" si="7"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -4436,19 +4883,23 @@
         <v>9</v>
       </c>
       <c r="D103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
       <c r="E103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1457672119140625E-6</v>
       </c>
       <c r="F103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1457672119140625</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <f t="shared" si="7"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -4459,19 +4910,23 @@
         <v>19</v>
       </c>
       <c r="D104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8388608</v>
       </c>
       <c r="E104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2649765014648438E-6</v>
       </c>
       <c r="F104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.2649765014648438</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <f t="shared" si="7"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -4482,19 +4937,23 @@
         <v>38</v>
       </c>
       <c r="D105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16777216</v>
       </c>
       <c r="E105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2649765014648438E-6</v>
       </c>
       <c r="F105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.2649765014648438</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <f t="shared" si="7"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -4505,20 +4964,25 @@
         <v>75</v>
       </c>
       <c r="D106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33554432</v>
       </c>
       <c r="E106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.2351741790771484E-6</v>
       </c>
       <c r="F106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.2351741790771484</v>
+      </c>
+      <c r="G106">
+        <f t="shared" si="7"/>
+        <v>134217728</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>